<commit_message>
Correção na Tabela de Pontuação
</commit_message>
<xml_diff>
--- a/src/data/pontuacao.xlsx
+++ b/src/data/pontuacao.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="52">
   <si>
     <t xml:space="preserve">LATTES</t>
   </si>
@@ -55,6 +55,9 @@
     <t xml:space="preserve">Nacional</t>
   </si>
   <si>
+    <t xml:space="preserve">VAZIO</t>
+  </si>
+  <si>
     <t xml:space="preserve">OUTRA-PRODUCAO-BIBLIOGRAFICA</t>
   </si>
   <si>
@@ -89,9 +92,6 @@
   </si>
   <si>
     <t xml:space="preserve">RESUMO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNDEF</t>
   </si>
   <si>
     <t xml:space="preserve">RESUMO_EXPANDIDO</t>
@@ -315,17 +315,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16:D31"/>
+      <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="36.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="43.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1017" min="4" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1017" min="5" style="0" width="8.67"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1018" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -365,6 +366,9 @@
       <c r="E2" s="0" t="n">
         <v>3.5</v>
       </c>
+      <c r="F2" s="0" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -382,30 +386,36 @@
       <c r="E3" s="0" t="n">
         <v>2.5</v>
       </c>
+      <c r="F3" s="0" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>2.5</v>
       </c>
+      <c r="F4" s="0" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -414,10 +424,10 @@
         <v>10</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>0.1</v>
+        <v>2.5</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>2</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -425,13 +435,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>0.1</v>
@@ -445,16 +455,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -462,7 +475,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>15</v>
@@ -471,7 +484,10 @@
         <v>10</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>0.5</v>
+        <v>0.2</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -479,7 +495,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>16</v>
@@ -488,7 +504,10 @@
         <v>10</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -496,7 +515,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>17</v>
@@ -508,7 +527,7 @@
         <v>0.1</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>2</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -516,7 +535,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>18</v>
@@ -536,10 +555,10 @@
         <v>6</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>10</v>
@@ -556,20 +575,19 @@
         <v>6</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="D13" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>1.5</v>
+        <v>0.1</v>
       </c>
       <c r="F13" s="0" t="n">
-        <f aca="false">E13*5</f>
-        <v>7.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -577,19 +595,20 @@
         <v>6</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>5</v>
+        <f aca="false">E14*5</f>
+        <v>7.5</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -597,19 +616,19 @@
         <v>6</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -617,36 +636,39 @@
         <v>6</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>2.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>2</v>
+        <v>0.5</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>2.5</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -654,16 +676,19 @@
         <v>25</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -671,16 +696,19 @@
         <v>25</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -688,16 +716,19 @@
         <v>25</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -705,33 +736,39 @@
         <v>25</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -739,16 +776,19 @@
         <v>34</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>4</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -759,13 +799,16 @@
         <v>37</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>4</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -776,13 +819,16 @@
         <v>37</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>4</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -790,16 +836,19 @@
         <v>34</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>4</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -807,16 +856,19 @@
         <v>34</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>4</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -824,16 +876,19 @@
         <v>34</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E28" s="0" t="n">
-        <v>2.5</v>
+        <v>4</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -841,19 +896,19 @@
         <v>34</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E29" s="0" t="n">
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
       <c r="F29" s="0" t="n">
-        <v>2</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -864,13 +919,16 @@
         <v>47</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>2.5</v>
+        <v>0.5</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -878,18 +936,38 @@
         <v>34</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E31" s="0" t="n">
+      <c r="D32" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F31" s="0" t="n">
+      <c r="F32" s="0" t="n">
         <v>16</v>
       </c>
     </row>

</xml_diff>